<commit_message>
Added genetic algorithm and some vis elements. Minor fixes.
</commit_message>
<xml_diff>
--- a/territories.xlsx
+++ b/territories.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="144">
   <si>
     <t>COLOMBIA</t>
   </si>
@@ -445,6 +445,12 @@
   </si>
   <si>
     <t>initial_factory</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -849,15 +855,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -879,8 +885,14 @@
       <c r="G1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -899,8 +911,14 @@
       <c r="F2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -919,8 +937,14 @@
       <c r="F3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>11</v>
+      </c>
+      <c r="I3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -939,8 +963,14 @@
       <c r="F4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>19</v>
+      </c>
+      <c r="I4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -959,8 +989,14 @@
       <c r="F5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -979,8 +1015,14 @@
       <c r="F6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -999,8 +1041,14 @@
       <c r="F7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1019,8 +1067,14 @@
       <c r="F8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1039,8 +1093,14 @@
       <c r="F9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1059,8 +1119,14 @@
       <c r="F10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1079,8 +1145,14 @@
       <c r="F11" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1099,8 +1171,14 @@
       <c r="F12" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>19</v>
+      </c>
+      <c r="I12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1119,8 +1197,14 @@
       <c r="F13" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13">
+        <v>24</v>
+      </c>
+      <c r="I13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -1139,8 +1223,14 @@
       <c r="F14" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14">
+        <v>21</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1159,8 +1249,14 @@
       <c r="F15" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15">
+        <v>22</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1179,8 +1275,14 @@
       <c r="F16" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1199,8 +1301,14 @@
       <c r="F17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17">
+        <v>34</v>
+      </c>
+      <c r="I17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1219,8 +1327,14 @@
       <c r="F18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="H18">
+        <v>34</v>
+      </c>
+      <c r="I18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1239,8 +1353,14 @@
       <c r="F19" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="H19">
+        <v>37</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1259,8 +1379,14 @@
       <c r="F20" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="H20">
+        <v>37</v>
+      </c>
+      <c r="I20">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1279,8 +1405,14 @@
       <c r="F21" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="H21">
+        <v>41</v>
+      </c>
+      <c r="I21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1299,8 +1431,14 @@
       <c r="F22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="H22">
+        <v>42</v>
+      </c>
+      <c r="I22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1319,8 +1457,14 @@
       <c r="F23" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="H23">
+        <v>43</v>
+      </c>
+      <c r="I23">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1339,8 +1483,14 @@
       <c r="F24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="H24">
+        <v>44</v>
+      </c>
+      <c r="I24">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1359,8 +1509,14 @@
       <c r="F25" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="H25">
+        <v>53</v>
+      </c>
+      <c r="I25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1379,8 +1535,14 @@
       <c r="F26" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="H26">
+        <v>63</v>
+      </c>
+      <c r="I26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1399,8 +1561,14 @@
       <c r="F27" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="H27">
+        <v>49</v>
+      </c>
+      <c r="I27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1419,8 +1587,14 @@
       <c r="F28" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="H28">
+        <v>57</v>
+      </c>
+      <c r="I28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1439,8 +1613,14 @@
       <c r="F29" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="H29">
+        <v>49</v>
+      </c>
+      <c r="I29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1459,8 +1639,14 @@
       <c r="F30" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="H30">
+        <v>54</v>
+      </c>
+      <c r="I30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1479,8 +1665,14 @@
       <c r="F31" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="H31">
+        <v>60</v>
+      </c>
+      <c r="I31">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -1499,8 +1691,14 @@
       <c r="F32" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="H32">
+        <v>59</v>
+      </c>
+      <c r="I32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1519,8 +1717,14 @@
       <c r="F33" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="H33">
+        <v>63</v>
+      </c>
+      <c r="I33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1539,8 +1743,14 @@
       <c r="F34" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="H34">
+        <v>64.5</v>
+      </c>
+      <c r="I34">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1559,8 +1769,14 @@
       <c r="F35" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="H35">
+        <v>67.5</v>
+      </c>
+      <c r="I35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1579,8 +1795,14 @@
       <c r="F36" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="H36">
+        <v>53</v>
+      </c>
+      <c r="I36">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -1599,8 +1821,14 @@
       <c r="F37" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="H37">
+        <v>52</v>
+      </c>
+      <c r="I37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -1619,8 +1847,14 @@
       <c r="F38" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="H38">
+        <v>56</v>
+      </c>
+      <c r="I38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -1639,8 +1873,14 @@
       <c r="F39" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="H39">
+        <v>54</v>
+      </c>
+      <c r="I39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -1659,8 +1899,14 @@
       <c r="F40" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="H40">
+        <v>60</v>
+      </c>
+      <c r="I40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1679,8 +1925,14 @@
       <c r="F41" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="H41">
+        <v>63</v>
+      </c>
+      <c r="I41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -1699,8 +1951,14 @@
       <c r="F42" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="H42">
+        <v>65</v>
+      </c>
+      <c r="I42">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -1719,8 +1977,14 @@
       <c r="F43" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="H43">
+        <v>67</v>
+      </c>
+      <c r="I43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1739,8 +2003,14 @@
       <c r="F44" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="H44">
+        <v>72</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -1759,8 +2029,14 @@
       <c r="F45" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="H45">
+        <v>47</v>
+      </c>
+      <c r="I45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1779,8 +2055,14 @@
       <c r="F46" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="H46">
+        <v>45</v>
+      </c>
+      <c r="I46">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>34</v>
       </c>
@@ -1799,8 +2081,14 @@
       <c r="F47" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="H47">
+        <v>37</v>
+      </c>
+      <c r="I47">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -1819,8 +2107,14 @@
       <c r="F48" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48">
+        <v>32</v>
+      </c>
+      <c r="I48">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -1839,8 +2133,14 @@
       <c r="F49" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49">
+        <v>37</v>
+      </c>
+      <c r="I49">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -1859,8 +2159,14 @@
       <c r="F50" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50">
+        <v>44</v>
+      </c>
+      <c r="I50">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -1879,8 +2185,14 @@
       <c r="F51" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51">
+        <v>39</v>
+      </c>
+      <c r="I51">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -1899,8 +2211,14 @@
       <c r="F52" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52">
+        <v>41</v>
+      </c>
+      <c r="I52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>40</v>
       </c>
@@ -1922,8 +2240,14 @@
       <c r="G53" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>41</v>
       </c>
@@ -1942,8 +2266,14 @@
       <c r="F54" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -1962,8 +2292,14 @@
       <c r="F55" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55">
+        <v>25</v>
+      </c>
+      <c r="I55">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -1985,8 +2321,14 @@
       <c r="G56" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56">
+        <v>22</v>
+      </c>
+      <c r="I56">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>44</v>
       </c>
@@ -2005,8 +2347,14 @@
       <c r="F57" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57">
+        <v>28</v>
+      </c>
+      <c r="I57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>45</v>
       </c>
@@ -2025,8 +2373,14 @@
       <c r="F58" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58">
+        <v>34</v>
+      </c>
+      <c r="I58">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>46</v>
       </c>
@@ -2048,8 +2402,14 @@
       <c r="G59" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59">
+        <v>39</v>
+      </c>
+      <c r="I59">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -2071,8 +2431,14 @@
       <c r="G60" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60">
+        <v>53</v>
+      </c>
+      <c r="I60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -2091,8 +2457,14 @@
       <c r="F61" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61">
+        <v>71</v>
+      </c>
+      <c r="I61">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>49</v>
       </c>
@@ -2111,8 +2483,14 @@
       <c r="F62" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62">
+        <v>70</v>
+      </c>
+      <c r="I62">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>97</v>
       </c>
@@ -2130,6 +2508,12 @@
       </c>
       <c r="F63" t="s">
         <v>111</v>
+      </c>
+      <c r="H63">
+        <v>65</v>
+      </c>
+      <c r="I63">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>